<commit_message>
everything is working fine with gemini + google sheet _ selenium
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/AirDoctorTestData.xlsx
+++ b/src/test/resources/testdata/AirDoctorTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MridulVashistha\eclipse-workspace\AirDoctorAutomationTest\src\test\resources\testdata\"/>
     </mc:Choice>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5000" uniqueCount="2697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5005" uniqueCount="2701">
   <si>
     <t>ModelName</t>
   </si>
@@ -8132,13 +8132,26 @@
   </si>
   <si>
     <t>https://airdoctorpro.com/?c=ewf07024</t>
+  </si>
+  <si>
+    <t>$629.00</t>
+  </si>
+  <si>
+    <t>$56.77</t>
+  </si>
+  <si>
+    <t>$685.77</t>
+  </si>
+  <si>
+    <t>288256</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8743,6 +8756,21 @@
       <c r="R2" s="9" t="s">
         <v>31</v>
       </c>
+      <c r="S2" t="s">
+        <v>2697</v>
+      </c>
+      <c r="T2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U2" t="s">
+        <v>2698</v>
+      </c>
+      <c r="V2" t="s">
+        <v>2699</v>
+      </c>
+      <c r="W2" t="s">
+        <v>2700</v>
+      </c>
     </row>
     <row r="3" spans="1:23" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -10063,7 +10091,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="53" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="53.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -20569,7 +20597,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="48.90625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -31075,7 +31103,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="47.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="47.26953125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -33021,7 +33049,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>